<commit_message>
Changed calc lemma proof for bous
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -506,7 +506,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -583,7 +583,7 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -813,7 +813,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Edited boussinesq--did analytic wp
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13560" tabRatio="500"/>
+    <workbookView xWindow="2740" yWindow="7740" windowWidth="21480" windowHeight="4600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="roster (2).csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Larme, Marye C.</t>
   </si>
@@ -136,12 +136,33 @@
   </si>
   <si>
     <t>Kopetsky, Emily G.</t>
+  </si>
+  <si>
+    <t>Exam 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW TOTAL</t>
+  </si>
+  <si>
+    <t>QUIZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOTAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -503,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -514,287 +535,741 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>95</v>
+      </c>
+      <c r="D2">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <f>ROUND(SUM(B2:E2)/295 * 100, 0)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>78</v>
+      </c>
+      <c r="D3">
+        <v>79</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F35" si="0">ROUND(SUM(B3:E3)/295 * 100, 0)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>98</v>
+      </c>
+      <c r="D4">
+        <v>78</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <v>78</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>77</v>
+      </c>
+      <c r="D8">
+        <v>78</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>85</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>72</v>
+      </c>
+      <c r="D10">
+        <v>74</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>79</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>28</v>
       </c>
       <c r="B12">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>69</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>79</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>77</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>71</v>
+      </c>
+      <c r="D16">
+        <v>52</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>75</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>77</v>
+      </c>
+      <c r="D18">
+        <v>79</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>73</v>
+      </c>
+      <c r="D19">
+        <v>73</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>71</v>
+      </c>
+      <c r="D20">
+        <v>66</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>78</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>72</v>
+      </c>
+      <c r="D22">
+        <v>75</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>71</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>74</v>
+      </c>
+      <c r="D24">
+        <v>74</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>64</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>78</v>
+      </c>
+      <c r="D26">
+        <v>76</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>83</v>
+      </c>
+      <c r="D27">
+        <v>77</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>80</v>
+      </c>
+      <c r="D29">
+        <v>77</v>
+      </c>
+      <c r="E29">
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>83</v>
+      </c>
+      <c r="D30">
+        <v>65</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>74</v>
+      </c>
+      <c r="D31">
+        <v>72</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>86</v>
+      </c>
+      <c r="D32">
+        <v>76</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>78</v>
+      </c>
+      <c r="E33">
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>71</v>
+      </c>
+      <c r="D34">
+        <v>78</v>
+      </c>
+      <c r="E34">
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C35">
+        <v>77</v>
+      </c>
+      <c r="D35">
+        <v>76</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -802,8 +1277,20 @@
         <f>MEDIAN(B2:B35)</f>
         <v>89.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <f>MEDIAN(C2:C35)</f>
+        <v>77</v>
+      </c>
+      <c r="D37">
+        <f>MEDIAN(D2:D35)</f>
+        <v>76</v>
+      </c>
+      <c r="F37">
+        <f>MEDIAN(F2:F35)</f>
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -811,10 +1298,24 @@
         <f>ROUNDUP(AVERAGE(B2:B35),1)</f>
         <v>87.5</v>
       </c>
+      <c r="C38">
+        <f>ROUNDUP(AVERAGE(C2:C35),1)</f>
+        <v>77</v>
+      </c>
+      <c r="D38">
+        <f>ROUNDUP(AVERAGE(D2:D35),1)</f>
+        <v>74.5</v>
+      </c>
+      <c r="F38">
+        <f>ROUNDUP(AVERAGE(F2:F35),1)</f>
+        <v>86.1</v>
+      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Changed boussinesq large data argument slightly
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="7740" windowWidth="21480" windowHeight="4600" tabRatio="500"/>
+    <workbookView xWindow="700" yWindow="840" windowWidth="21480" windowHeight="4600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="roster (2).csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Larme, Marye C.</t>
   </si>
@@ -150,6 +150,10 @@
   </si>
   <si>
     <t>TOTAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Participation and Activities</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,18 +528,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -554,8 +559,11 @@
       <c r="F1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -575,8 +583,11 @@
         <f>ROUND(SUM(B2:E2)/295 * 100, 0)</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -596,8 +607,11 @@
         <f t="shared" ref="F3:F35" si="0">ROUND(SUM(B3:E3)/295 * 100, 0)</f>
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -617,8 +631,11 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -638,8 +655,11 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -659,8 +679,11 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -680,8 +703,11 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -701,8 +727,11 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -722,8 +751,11 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -743,8 +775,11 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -764,8 +799,11 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -785,8 +823,11 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -806,8 +847,11 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -827,8 +871,11 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -848,8 +895,11 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -869,8 +919,11 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -890,8 +943,11 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -911,8 +967,11 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -932,8 +991,11 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -953,8 +1015,11 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -974,8 +1039,11 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -995,8 +1063,11 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1016,8 +1087,11 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1037,8 +1111,11 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1058,8 +1135,11 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1079,8 +1159,11 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1100,8 +1183,11 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1121,8 +1207,11 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1142,8 +1231,11 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1163,8 +1255,11 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1184,8 +1279,11 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1205,8 +1303,11 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1226,8 +1327,11 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1247,8 +1351,11 @@
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1268,8 +1375,11 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1290,7 +1400,7 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1312,7 +1422,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
some more bous changes
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Larme, Marye C.</t>
   </si>
@@ -61,10 +61,6 @@
   </si>
   <si>
     <t>Yoo, Dong Suk</t>
-  </si>
-  <si>
-    <t>Exam 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Median</t>
@@ -138,10 +134,6 @@
     <t>Kopetsky, Emily G.</t>
   </si>
   <si>
-    <t>Exam 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HW TOTAL</t>
   </si>
   <si>
@@ -153,7 +145,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Participation and Activities</t>
+    <t>PACT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXAM 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXAM 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXAM 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,44 +532,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>18</v>
       </c>
       <c r="B2">
         <v>66</v>
@@ -574,22 +581,25 @@
         <v>95</v>
       </c>
       <c r="D2">
+        <v>84</v>
+      </c>
+      <c r="E2">
         <v>74</v>
       </c>
-      <c r="E2">
-        <v>15</v>
-      </c>
       <c r="F2">
-        <f>ROUND(SUM(B2:E2)/295 * 100, 0)</f>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <f>ROUND(SUM(B2:G2)/295 * 100, 0)</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>98</v>
@@ -598,22 +608,25 @@
         <v>78</v>
       </c>
       <c r="D3">
+        <v>99</v>
+      </c>
+      <c r="E3">
         <v>79</v>
       </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
       <c r="F3">
-        <f t="shared" ref="F3:F35" si="0">ROUND(SUM(B3:E3)/295 * 100, 0)</f>
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <f t="shared" ref="H3:H35" si="0">ROUND(SUM(B3:G3)/295 * 100, 0)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>99</v>
@@ -622,22 +635,25 @@
         <v>98</v>
       </c>
       <c r="D4">
+        <v>83</v>
+      </c>
+      <c r="E4">
         <v>78</v>
       </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>86</v>
@@ -646,22 +662,25 @@
         <v>93</v>
       </c>
       <c r="D5">
+        <v>94</v>
+      </c>
+      <c r="E5">
         <v>78</v>
       </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -670,22 +689,25 @@
         <v>90</v>
       </c>
       <c r="D6">
+        <v>93</v>
+      </c>
+      <c r="E6">
         <v>75</v>
       </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>89</v>
@@ -694,22 +716,25 @@
         <v>72</v>
       </c>
       <c r="D7">
+        <v>85</v>
+      </c>
+      <c r="E7">
         <v>74</v>
       </c>
-      <c r="E7">
-        <v>15</v>
-      </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -718,22 +743,25 @@
         <v>77</v>
       </c>
       <c r="D8">
+        <v>89</v>
+      </c>
+      <c r="E8">
         <v>78</v>
       </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -742,22 +770,25 @@
         <v>85</v>
       </c>
       <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
         <v>80</v>
       </c>
-      <c r="E9">
-        <v>15</v>
-      </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>78</v>
@@ -766,22 +797,25 @@
         <v>72</v>
       </c>
       <c r="D10">
+        <v>83</v>
+      </c>
+      <c r="E10">
         <v>74</v>
       </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>91</v>
@@ -790,22 +824,25 @@
         <v>80</v>
       </c>
       <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
         <v>79</v>
       </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="G11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>87</v>
@@ -814,22 +851,25 @@
         <v>64</v>
       </c>
       <c r="D12">
+        <v>84</v>
+      </c>
+      <c r="E12">
         <v>76</v>
       </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>93</v>
@@ -838,22 +878,25 @@
         <v>69</v>
       </c>
       <c r="D13">
+        <v>91</v>
+      </c>
+      <c r="E13">
         <v>69</v>
       </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>99</v>
@@ -862,22 +905,25 @@
         <v>83</v>
       </c>
       <c r="D14">
+        <v>99</v>
+      </c>
+      <c r="E14">
         <v>79</v>
       </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>79</v>
@@ -886,22 +932,25 @@
         <v>50</v>
       </c>
       <c r="D15">
+        <v>93</v>
+      </c>
+      <c r="E15">
         <v>77</v>
       </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>78</v>
@@ -913,19 +962,22 @@
         <v>52</v>
       </c>
       <c r="E16">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>71</v>
@@ -934,22 +986,25 @@
         <v>68</v>
       </c>
       <c r="D17">
+        <v>80</v>
+      </c>
+      <c r="E17">
         <v>75</v>
       </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
       <c r="F17">
-        <f t="shared" si="0"/>
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>98</v>
@@ -958,22 +1013,25 @@
         <v>77</v>
       </c>
       <c r="D18">
+        <v>98</v>
+      </c>
+      <c r="E18">
         <v>79</v>
       </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>80</v>
@@ -982,22 +1040,25 @@
         <v>73</v>
       </c>
       <c r="D19">
+        <v>74</v>
+      </c>
+      <c r="E19">
         <v>73</v>
       </c>
-      <c r="E19">
-        <v>15</v>
-      </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>76</v>
@@ -1006,22 +1067,25 @@
         <v>71</v>
       </c>
       <c r="D20">
+        <v>83</v>
+      </c>
+      <c r="E20">
         <v>66</v>
       </c>
-      <c r="E20">
-        <v>15</v>
-      </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>96</v>
@@ -1030,20 +1094,23 @@
         <v>68</v>
       </c>
       <c r="D21">
+        <v>97</v>
+      </c>
+      <c r="E21">
         <v>78</v>
       </c>
-      <c r="E21">
-        <v>15</v>
-      </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="G21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1054,20 +1121,23 @@
         <v>72</v>
       </c>
       <c r="D22">
+        <v>70</v>
+      </c>
+      <c r="E22">
         <v>75</v>
       </c>
-      <c r="E22">
-        <v>15</v>
-      </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="G22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1078,20 +1148,23 @@
         <v>71</v>
       </c>
       <c r="D23">
+        <v>80</v>
+      </c>
+      <c r="E23">
         <v>75</v>
       </c>
-      <c r="E23">
-        <v>15</v>
-      </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="G23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1102,20 +1175,23 @@
         <v>74</v>
       </c>
       <c r="D24">
+        <v>94</v>
+      </c>
+      <c r="E24">
         <v>74</v>
       </c>
-      <c r="E24">
-        <v>15</v>
-      </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1126,20 +1202,23 @@
         <v>43</v>
       </c>
       <c r="D25">
+        <v>72</v>
+      </c>
+      <c r="E25">
         <v>64</v>
       </c>
-      <c r="E25">
-        <v>15</v>
-      </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="G25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1150,20 +1229,23 @@
         <v>78</v>
       </c>
       <c r="D26">
+        <v>93</v>
+      </c>
+      <c r="E26">
         <v>76</v>
       </c>
-      <c r="E26">
-        <v>15</v>
-      </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="G26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1174,20 +1256,23 @@
         <v>83</v>
       </c>
       <c r="D27">
+        <v>69</v>
+      </c>
+      <c r="E27">
         <v>77</v>
       </c>
-      <c r="E27">
-        <v>15</v>
-      </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1198,20 +1283,23 @@
         <v>90</v>
       </c>
       <c r="D28">
+        <v>98</v>
+      </c>
+      <c r="E28">
         <v>75</v>
       </c>
-      <c r="E28">
-        <v>15</v>
-      </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="G28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1222,20 +1310,23 @@
         <v>80</v>
       </c>
       <c r="D29">
+        <v>83</v>
+      </c>
+      <c r="E29">
         <v>77</v>
       </c>
-      <c r="E29">
-        <v>15</v>
-      </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="G29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1246,20 +1337,23 @@
         <v>83</v>
       </c>
       <c r="D30">
+        <v>83</v>
+      </c>
+      <c r="E30">
         <v>65</v>
       </c>
-      <c r="E30">
-        <v>15</v>
-      </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1270,20 +1364,23 @@
         <v>74</v>
       </c>
       <c r="D31">
+        <v>71</v>
+      </c>
+      <c r="E31">
         <v>72</v>
       </c>
-      <c r="E31">
-        <v>15</v>
-      </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1294,20 +1391,23 @@
         <v>86</v>
       </c>
       <c r="D32">
+        <v>99</v>
+      </c>
+      <c r="E32">
         <v>76</v>
       </c>
-      <c r="E32">
-        <v>15</v>
-      </c>
       <c r="F32">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="G32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1318,20 +1418,23 @@
         <v>100</v>
       </c>
       <c r="D33">
+        <v>88</v>
+      </c>
+      <c r="E33">
         <v>78</v>
       </c>
-      <c r="E33">
-        <v>15</v>
-      </c>
       <c r="F33">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1342,20 +1445,23 @@
         <v>71</v>
       </c>
       <c r="D34">
+        <v>76</v>
+      </c>
+      <c r="E34">
         <v>78</v>
       </c>
-      <c r="E34">
-        <v>15</v>
-      </c>
       <c r="F34">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1366,22 +1472,25 @@
         <v>77</v>
       </c>
       <c r="D35">
+        <v>97</v>
+      </c>
+      <c r="E35">
         <v>76</v>
       </c>
-      <c r="E35">
-        <v>15</v>
-      </c>
       <c r="F35">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="G35">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37">
         <f>MEDIAN(B2:B35)</f>
@@ -1393,16 +1502,28 @@
       </c>
       <c r="D37">
         <f>MEDIAN(D2:D35)</f>
+        <v>86.5</v>
+      </c>
+      <c r="E37">
+        <f>MEDIAN(E2:E35)</f>
         <v>76</v>
       </c>
       <c r="F37">
         <f>MEDIAN(F2:F35)</f>
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <f>MEDIAN(G2:G35)</f>
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <f>MEDIAN(H2:H35)</f>
+        <v>115.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38">
         <f>ROUNDUP(AVERAGE(B2:B35),1)</f>
@@ -1414,14 +1535,27 @@
       </c>
       <c r="D38">
         <f>ROUNDUP(AVERAGE(D2:D35),1)</f>
+        <v>86.199999999999989</v>
+      </c>
+      <c r="E38">
+        <f>ROUNDUP(AVERAGE(E2:E35),1)</f>
         <v>74.5</v>
       </c>
       <c r="F38">
         <f>ROUNDUP(AVERAGE(F2:F35),1)</f>
-        <v>86.1</v>
+        <v>15</v>
+      </c>
+      <c r="G38">
+        <f>ROUNDUP(AVERAGE(G2:G35),1)</f>
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <f>ROUNDUP(AVERAGE(H2:H35),1)</f>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Traveling wave document before getting rid of c in computations
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -165,12 +165,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -535,7 +529,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1472,7 +1466,7 @@
         <v>77</v>
       </c>
       <c r="D35">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E35">
         <v>76</v>
@@ -1493,31 +1487,31 @@
         <v>14</v>
       </c>
       <c r="B37">
-        <f>MEDIAN(B2:B35)</f>
+        <f t="shared" ref="B37:H37" si="1">MEDIAN(B2:B35)</f>
         <v>89.5</v>
       </c>
       <c r="C37">
-        <f>MEDIAN(C2:C35)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="D37">
-        <f>MEDIAN(D2:D35)</f>
+        <f t="shared" si="1"/>
         <v>86.5</v>
       </c>
       <c r="E37">
-        <f>MEDIAN(E2:E35)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="F37">
-        <f>MEDIAN(F2:F35)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G37">
-        <f>MEDIAN(G2:G35)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H37">
-        <f>MEDIAN(H2:H35)</f>
+        <f t="shared" si="1"/>
         <v>115.5</v>
       </c>
     </row>
@@ -1526,39 +1520,37 @@
         <v>15</v>
       </c>
       <c r="B38">
-        <f>ROUNDUP(AVERAGE(B2:B35),1)</f>
+        <f t="shared" ref="B38:H38" si="2">ROUNDUP(AVERAGE(B2:B35),1)</f>
         <v>87.5</v>
       </c>
       <c r="C38">
-        <f>ROUNDUP(AVERAGE(C2:C35),1)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="D38">
-        <f>ROUNDUP(AVERAGE(D2:D35),1)</f>
-        <v>86.199999999999989</v>
+        <f t="shared" si="2"/>
+        <v>86.3</v>
       </c>
       <c r="E38">
-        <f>ROUNDUP(AVERAGE(E2:E35),1)</f>
+        <f t="shared" si="2"/>
         <v>74.5</v>
       </c>
       <c r="F38">
-        <f>ROUNDUP(AVERAGE(F2:F35),1)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G38">
-        <f>ROUNDUP(AVERAGE(G2:G35),1)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="H38">
-        <f>ROUNDUP(AVERAGE(H2:H35),1)</f>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
more trave wave changes
</commit_message>
<xml_diff>
--- a/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
+++ b/teaching/m10260/spr-11/grades-m10260-sp11.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Larme, Marye C.</t>
   </si>
@@ -158,6 +158,10 @@
   </si>
   <si>
     <t>EXAM 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROJECTS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -165,6 +169,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -526,19 +536,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="7" max="8" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -561,10 +571,13 @@
         <v>40</v>
       </c>
       <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -587,11 +600,14 @@
         <v>5</v>
       </c>
       <c r="H2">
-        <f>ROUND(SUM(B2:G2)/295 * 100, 0)</f>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <f>ROUND(SUM(B2:H2)/295 * 100, 0)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -614,11 +630,14 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H35" si="0">ROUND(SUM(B3:G3)/295 * 100, 0)</f>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I35" si="0">ROUND(SUM(B3:H3)/295 * 100, 0)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -641,11 +660,14 @@
         <v>5</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -668,11 +690,14 @@
         <v>5</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -695,11 +720,14 @@
         <v>5</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -722,11 +750,14 @@
         <v>5</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -749,11 +780,14 @@
         <v>5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -776,11 +810,14 @@
         <v>5</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -803,11 +840,14 @@
         <v>5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -830,11 +870,14 @@
         <v>5</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -857,11 +900,14 @@
         <v>5</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -884,11 +930,14 @@
         <v>5</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -911,11 +960,14 @@
         <v>5</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -938,11 +990,14 @@
         <v>5</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -965,11 +1020,14 @@
         <v>5</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -992,11 +1050,14 @@
         <v>5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1019,11 +1080,14 @@
         <v>5</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1046,11 +1110,14 @@
         <v>5</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1073,11 +1140,14 @@
         <v>5</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1100,11 +1170,14 @@
         <v>5</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1127,11 +1200,14 @@
         <v>5</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1154,11 +1230,14 @@
         <v>5</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1181,11 +1260,14 @@
         <v>5</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1208,11 +1290,14 @@
         <v>5</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1235,11 +1320,14 @@
         <v>5</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1262,11 +1350,14 @@
         <v>5</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1289,11 +1380,14 @@
         <v>5</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1316,11 +1410,14 @@
         <v>5</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1343,11 +1440,14 @@
         <v>5</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1370,11 +1470,14 @@
         <v>5</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1397,11 +1500,14 @@
         <v>5</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1424,11 +1530,14 @@
         <v>5</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1451,11 +1560,14 @@
         <v>5</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1478,16 +1590,19 @@
         <v>5</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:H37" si="1">MEDIAN(B2:B35)</f>
+        <f t="shared" ref="B37:I38" si="1">MEDIAN(B2:B35)</f>
         <v>89.5</v>
       </c>
       <c r="C37">
@@ -1512,15 +1627,19 @@
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>115.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>120.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="B38">
-        <f t="shared" ref="B38:H38" si="2">ROUNDUP(AVERAGE(B2:B35),1)</f>
+        <f t="shared" ref="B38:I38" si="2">ROUNDUP(AVERAGE(B2:B35),1)</f>
         <v>87.5</v>
       </c>
       <c r="C38">
@@ -1545,12 +1664,17 @@
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>117</v>
+        <v>14.2</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>121.8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>